<commit_message>
Update Check List Actividades PF - ML.xlsx
</commit_message>
<xml_diff>
--- a/data/raw/Check List Actividades PF - ML.xlsx
+++ b/data/raw/Check List Actividades PF - ML.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salva\Desktop\my_ml_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salva\Documents\GitHub\ml_default_credit_card_clients\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E10B4DD-D1A0-4D7B-B12E-812322677D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0179E4E-6BAF-48D9-B6DA-E61113067938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{67AF5B1A-1E2B-4CAA-9A64-6693CB82A0D1}"/>
   </bookViews>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3614DB83-2EAA-491F-9B2C-AF13CF2011A9}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B6" sqref="A6:B13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +634,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -650,7 +650,7 @@
         <v>20</v>
       </c>
       <c r="B4" s="6">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
EDA Final antes de retroalimentación
</commit_message>
<xml_diff>
--- a/data/raw/Check List Actividades PF - ML.xlsx
+++ b/data/raw/Check List Actividades PF - ML.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salva\Documents\GitHub\ml_default_credit_card_clients\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED1EA22-125B-4F31-9C28-A7D8B49146CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18472B6E-9C6D-4A3E-8858-A7F37AD5908A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{67AF5B1A-1E2B-4CAA-9A64-6693CB82A0D1}"/>
   </bookViews>
@@ -335,27 +335,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -381,6 +360,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -402,16 +402,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8943705F-C6D8-4865-AA83-51A9FFC69472}" name="Tabla1" displayName="Tabla1" ref="A1:E39" totalsRowCount="1">
   <autoFilter ref="A1:E38" xr:uid="{8943705F-C6D8-4865-AA83-51A9FFC69472}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{237A710D-016B-4979-9DA7-41FFFD27973E}" name="Actividades" dataDxfId="6" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{0838B906-08D4-41C1-BF83-F676F0BED85A}" name="Estatus" dataDxfId="5" totalsRowDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{91E29D4E-59B1-4C8A-8940-0F901C526952}" name="Avance" totalsRowFunction="custom" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{237A710D-016B-4979-9DA7-41FFFD27973E}" name="Actividades" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{0838B906-08D4-41C1-BF83-F676F0BED85A}" name="Estatus" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{91E29D4E-59B1-4C8A-8940-0F901C526952}" name="Avance" totalsRowFunction="custom" dataDxfId="2">
       <calculatedColumnFormula>+IF(Tabla1[[#This Row],[Estatus]]=1,1,0)</calculatedColumnFormula>
       <totalsRowFormula>+SUM(Tabla1[Avance])</totalsRowFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{56694461-29B6-4DEB-B183-B64D7B410F39}" name="Total actividades" totalsRowFunction="custom">
       <totalsRowFormula>+SUM(Tabla1[Total actividades])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B16F3491-FCB9-44DB-97FD-F594D944B4BB}" name="Avance %" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="0" dataCellStyle="Porcentaje">
+    <tableColumn id="5" xr3:uid="{B16F3491-FCB9-44DB-97FD-F594D944B4BB}" name="Avance %" totalsRowFunction="custom" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>+Tabla1[[#This Row],[Avance]]/Tabla1[[#This Row],[Total actividades]]</calculatedColumnFormula>
       <totalsRowFormula>Tabla1[[#Totals],[Avance]]/Tabla1[[#Totals],[Total actividades]]</totalsRowFormula>
     </tableColumn>
@@ -720,7 +720,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>